<commit_message>
review of HearingFunction, made some fixes already
</commit_message>
<xml_diff>
--- a/Mappings/HearingFunction - STU3.xlsx
+++ b/Mappings/HearingFunction - STU3.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edelman\Nictiz-STU3-Zib2017\Mappings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\nictiz-stu3-zib2017\Mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D3545A-988F-4ECA-9701-31B13DE91199}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="182">
   <si>
     <t>Subject</t>
   </si>
@@ -238,9 +237,6 @@
     <t>Reference</t>
   </si>
   <si>
-    <t>Constraints</t>
-  </si>
-  <si>
     <t>HearingFunction</t>
   </si>
   <si>
@@ -484,9 +480,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>nl-core-observation</t>
-  </si>
-  <si>
     <t>.valueCodeableConcept</t>
   </si>
   <si>
@@ -572,13 +565,22 @@
   </si>
   <si>
     <t>The valueset includes the option 'none' ('geen'), which maps somewhat poorly onto the MedicalDevice/MedicalDeveiceProduct approach, which is based on the premise that an aid is present.</t>
+  </si>
+  <si>
+    <t>Zulip chats</t>
+  </si>
+  <si>
+    <t>https://chat.fhir.org/#narrow/stream/179166-implementers/topic/Modeling.20Hearing.2FVisual.20Function</t>
+  </si>
+  <si>
+    <t>Observation (derived from nl-core-observation)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
@@ -616,6 +618,12 @@
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="5">
@@ -702,8 +710,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -755,15 +764,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2911,18 +2919,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2930,7 +2938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:3">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -2938,7 +2946,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:3">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -2946,7 +2954,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:3">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
@@ -2954,7 +2962,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:3">
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -2962,7 +2970,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:3">
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
@@ -2970,7 +2978,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:3">
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
@@ -2978,7 +2986,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:3">
       <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
@@ -2986,7 +2994,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:3">
       <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
@@ -2994,7 +3002,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:3">
       <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
@@ -3002,7 +3010,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:3" ht="38.25">
       <c r="B12" s="2" t="s">
         <v>55</v>
       </c>
@@ -3010,7 +3018,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:3" ht="25.5">
       <c r="B13" s="2" t="s">
         <v>57</v>
       </c>
@@ -3018,7 +3026,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:3">
       <c r="B14" s="2" t="s">
         <v>59</v>
       </c>
@@ -3028,7 +3036,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C11" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -3039,24 +3047,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="2" max="2" width="35" customWidth="1"/>
     <col min="3" max="3" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="20" t="s">
+    <row r="2" spans="2:3">
+      <c r="B2" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="20"/>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C2" s="19"/>
+    </row>
+    <row r="3" spans="2:3">
       <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
@@ -3064,7 +3072,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:3">
       <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
@@ -3072,7 +3080,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:3">
       <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
@@ -3080,7 +3088,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:3">
       <c r="B6" s="2" t="s">
         <v>26</v>
       </c>
@@ -3088,7 +3096,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:3">
       <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
@@ -3096,7 +3104,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:3">
       <c r="B8" s="2" t="s">
         <v>28</v>
       </c>
@@ -3104,13 +3112,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:3">
       <c r="B9" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:3">
       <c r="B10" s="2" t="s">
         <v>31</v>
       </c>
@@ -3118,13 +3126,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:3">
       <c r="B11" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:3">
       <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
@@ -3132,13 +3140,13 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:3">
       <c r="B13" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:3">
       <c r="B14" s="2" t="s">
         <v>37</v>
       </c>
@@ -3146,7 +3154,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:3">
       <c r="B15" s="2" t="s">
         <v>39</v>
       </c>
@@ -3154,7 +3162,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:3">
       <c r="B16" s="2" t="s">
         <v>41</v>
       </c>
@@ -3162,7 +3170,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3">
       <c r="B17" s="2" t="s">
         <v>42</v>
       </c>
@@ -3170,7 +3178,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:3">
       <c r="B18" s="2" t="s">
         <v>43</v>
       </c>
@@ -3178,7 +3186,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:3">
       <c r="B19" s="2" t="s">
         <v>45</v>
       </c>
@@ -3186,7 +3194,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:3">
       <c r="B20" s="2" t="s">
         <v>46</v>
       </c>
@@ -3194,7 +3202,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:3">
       <c r="B21" s="2" t="s">
         <v>47</v>
       </c>
@@ -3202,7 +3210,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:3">
       <c r="B22" s="2" t="s">
         <v>49</v>
       </c>
@@ -3210,7 +3218,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:3">
       <c r="B23" s="2" t="s">
         <v>50</v>
       </c>
@@ -3218,7 +3226,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:3">
       <c r="B24" s="2" t="s">
         <v>52</v>
       </c>
@@ -3226,7 +3234,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:3">
       <c r="B25" s="2" t="s">
         <v>53</v>
       </c>
@@ -3246,14 +3254,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" s="2"/>
     </row>
   </sheetData>
@@ -3263,116 +3271,125 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AA401AD-53BB-460C-AC8C-35EFEDED25FD}">
-  <dimension ref="A1:J10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="51.140625" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
     <col min="6" max="6" width="15.140625" customWidth="1"/>
     <col min="7" max="7" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>154</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>156</v>
       </c>
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
       <c r="F1" s="16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G1" s="16"/>
       <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="17" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="C2" t="s">
-        <v>171</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="17" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
+    <row r="6" spans="1:8">
+      <c r="A6" s="17" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
+    <row r="7" spans="1:8">
+      <c r="A7" s="17" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
+    <row r="8" spans="1:8">
+      <c r="A8" s="17" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="17" t="s">
+      <c r="C8" t="s">
+        <v>168</v>
+      </c>
+      <c r="F8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="17" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
+      <c r="C9" t="s">
+        <v>166</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="C8" t="s">
-        <v>170</v>
-      </c>
-      <c r="F8" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="17" t="s">
-        <v>165</v>
-      </c>
-      <c r="C9" t="s">
-        <v>168</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
-        <v>166</v>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>179</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B17" r:id="rId1" location="narrow/stream/179166-implementers/topic/Modeling.20Hearing.2FVisual.20Function" display="https://chat.fhir.org/ - narrow/stream/179166-implementers/topic/Modeling.20Hearing.2FVisual.20Function"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x14">
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3073" r:id="rId4" name="Check Box 1">
+            <control shapeId="3073" r:id="rId5" name="Check Box 1">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3394,7 +3411,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3074" r:id="rId5" name="Check Box 2">
+            <control shapeId="3074" r:id="rId6" name="Check Box 2">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3416,7 +3433,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3075" r:id="rId6" name="Check Box 3">
+            <control shapeId="3075" r:id="rId7" name="Check Box 3">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3438,7 +3455,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3076" r:id="rId7" name="Check Box 4">
+            <control shapeId="3076" r:id="rId8" name="Check Box 4">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3460,7 +3477,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3077" r:id="rId8" name="Check Box 5">
+            <control shapeId="3077" r:id="rId9" name="Check Box 5">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3482,7 +3499,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3078" r:id="rId9" name="Check Box 6">
+            <control shapeId="3078" r:id="rId10" name="Check Box 6">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3504,7 +3521,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3079" r:id="rId10" name="Check Box 7">
+            <control shapeId="3079" r:id="rId11" name="Check Box 7">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3526,7 +3543,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3080" r:id="rId11" name="Check Box 8">
+            <control shapeId="3080" r:id="rId12" name="Check Box 8">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3548,7 +3565,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3081" r:id="rId12" name="Check Box 9">
+            <control shapeId="3081" r:id="rId13" name="Check Box 9">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3570,7 +3587,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3082" r:id="rId13" name="Check Box 10">
+            <control shapeId="3082" r:id="rId14" name="Check Box 10">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3592,7 +3609,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3083" r:id="rId14" name="Check Box 11">
+            <control shapeId="3083" r:id="rId15" name="Check Box 11">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3614,7 +3631,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3084" r:id="rId15" name="Check Box 12">
+            <control shapeId="3084" r:id="rId16" name="Check Box 12">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3636,7 +3653,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3085" r:id="rId16" name="Check Box 13">
+            <control shapeId="3085" r:id="rId17" name="Check Box 13">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3658,7 +3675,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3086" r:id="rId17" name="Check Box 14">
+            <control shapeId="3086" r:id="rId18" name="Check Box 14">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3680,7 +3697,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3087" r:id="rId18" name="Check Box 15">
+            <control shapeId="3087" r:id="rId19" name="Check Box 15">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3702,7 +3719,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3088" r:id="rId19" name="Check Box 16">
+            <control shapeId="3088" r:id="rId20" name="Check Box 16">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3724,7 +3741,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3089" r:id="rId20" name="Check Box 17">
+            <control shapeId="3089" r:id="rId21" name="Check Box 17">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3746,7 +3763,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3090" r:id="rId21" name="Check Box 18">
+            <control shapeId="3090" r:id="rId22" name="Check Box 18">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3768,7 +3785,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3091" r:id="rId22" name="Check Box 19">
+            <control shapeId="3091" r:id="rId23" name="Check Box 19">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3790,7 +3807,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3092" r:id="rId23" name="Check Box 20">
+            <control shapeId="3092" r:id="rId24" name="Check Box 20">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3812,7 +3829,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3093" r:id="rId24" name="Check Box 21">
+            <control shapeId="3093" r:id="rId25" name="Check Box 21">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3834,7 +3851,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3094" r:id="rId25" name="Check Box 22">
+            <control shapeId="3094" r:id="rId26" name="Check Box 22">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3856,7 +3873,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3095" r:id="rId26" name="Check Box 23">
+            <control shapeId="3095" r:id="rId27" name="Check Box 23">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3878,7 +3895,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3096" r:id="rId27" name="Check Box 24">
+            <control shapeId="3096" r:id="rId28" name="Check Box 24">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3905,14 +3922,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B2:T8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="2" max="6" width="2" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
@@ -3926,10 +3943,9 @@
     <col min="17" max="17" width="14.140625" customWidth="1"/>
     <col min="18" max="18" width="12.85546875" customWidth="1"/>
     <col min="19" max="19" width="30" customWidth="1"/>
-    <col min="20" max="20" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:19" ht="25.5">
       <c r="B2" s="5" t="s">
         <v>55</v>
       </c>
@@ -3963,24 +3979,21 @@
         <v>68</v>
       </c>
       <c r="P2" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q2" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="R2" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="Q2" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="R2" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="T2" s="1" t="s">
+    </row>
+    <row r="3" spans="2:19" ht="38.25">
+      <c r="B3" s="8" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B3" s="8" t="s">
-        <v>70</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -3988,248 +4001,242 @@
       <c r="F3" s="9"/>
       <c r="G3" s="10"/>
       <c r="H3" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L3" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="M3" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
       <c r="P3" s="4" t="s">
-        <v>151</v>
+        <v>181</v>
       </c>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
       <c r="S3" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="T3" s="4"/>
-    </row>
-    <row r="4" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" ht="25.5">
       <c r="B4" s="11"/>
       <c r="C4" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
       <c r="G4" s="13"/>
       <c r="H4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="O4" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="O4" s="3" t="s">
-        <v>82</v>
-      </c>
       <c r="P4" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="R4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="S4" s="3"/>
-      <c r="T4" s="2"/>
-    </row>
-    <row r="5" spans="2:20" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="2:19" ht="51">
       <c r="B5" s="11"/>
       <c r="C5" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
       <c r="G5" s="13"/>
       <c r="H5" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="O5" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="O5" s="3" t="s">
-        <v>90</v>
-      </c>
       <c r="P5" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
       <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-    </row>
-    <row r="6" spans="2:20" ht="76.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="2:19" ht="76.5">
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
       <c r="E6" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F6" s="12"/>
       <c r="G6" s="13"/>
       <c r="H6" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L6" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="M6" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="R6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="T6" s="2"/>
-    </row>
-    <row r="7" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" ht="38.25">
       <c r="B7" s="11"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
       <c r="E7" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="13"/>
       <c r="H7" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L7" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M7" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="N7" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="O7" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="O7" s="3" t="s">
-        <v>101</v>
-      </c>
       <c r="P7" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="R7" s="2" t="s">
         <v>2</v>
       </c>
       <c r="S7" s="3"/>
-      <c r="T7" s="19"/>
-    </row>
-    <row r="8" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="2:19" ht="25.5">
       <c r="B8" s="11"/>
       <c r="C8" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
       <c r="G8" s="13"/>
       <c r="H8" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="L8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="N8" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="O8" s="2"/>
       <c r="P8" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O4" location="HearingFunctionCodelist!A1" display="HearingFunctionCodelist" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="O5" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="O6" location="HearingAidTypeCodelist!A1" display="HearingAidTypeCodelist" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink ref="O7" location="DeviceAnatomicalLocationCodelis!A1" display="DeviceAnatomicalLocationCodelist" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="O4" location="HearingFunctionCodelist!A1" display="HearingFunctionCodelist"/>
+    <hyperlink ref="O5" r:id="rId1"/>
+    <hyperlink ref="O6" location="HearingAidTypeCodelist!A1" display="HearingAidTypeCodelist"/>
+    <hyperlink ref="O7" location="DeviceAnatomicalLocationCodelis!A1" display="DeviceAnatomicalLocationCodelist"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -4240,12 +4247,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -4254,83 +4261,83 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C3" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20" t="s">
+    <row r="3" spans="3:7">
+      <c r="C3" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+    </row>
+    <row r="4" spans="3:7">
+      <c r="C4" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-    </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C4" s="14" t="s">
+      <c r="D4" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="E4" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="F4" s="14" t="s">
         <v>112</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>113</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:7">
       <c r="C5" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="G5" s="2" t="s">
+    </row>
+    <row r="6" spans="3:7">
+      <c r="C6" s="2" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E6" s="2" t="s">
+    </row>
+    <row r="7" spans="3:7">
+      <c r="C7" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C7" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -4346,12 +4353,12 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -4360,66 +4367,66 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C3" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20" t="s">
-        <v>125</v>
-      </c>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-    </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:7">
+      <c r="C3" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+    </row>
+    <row r="4" spans="3:7">
       <c r="C4" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="E4" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="F4" s="14" t="s">
         <v>112</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>113</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:7" ht="25.5">
       <c r="C5" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7">
+      <c r="C6" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -4435,12 +4442,12 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -4449,83 +4456,83 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C3" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-    </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:7">
+      <c r="C3" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+    </row>
+    <row r="4" spans="3:7">
       <c r="C4" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="E4" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="F4" s="14" t="s">
         <v>112</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>113</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:7">
       <c r="C5" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E5" s="2" t="s">
+    </row>
+    <row r="6" spans="3:7">
+      <c r="C6" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C6" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E6" s="2" t="s">
+    </row>
+    <row r="7" spans="3:7">
+      <c r="C7" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C7" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -4541,44 +4548,44 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="2" max="2" width="150" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:2">
       <c r="B2" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" ht="140.25">
+      <c r="B3" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="2:2" ht="140.25" x14ac:dyDescent="0.2">
-      <c r="B3" s="2" t="s">
+    <row r="4" spans="2:2">
+      <c r="B4" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B4" s="1" t="s">
+    <row r="5" spans="2:2" ht="25.5">
+      <c r="B5" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B5" s="2" t="s">
+    <row r="6" spans="2:2">
+      <c r="B6" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B6" s="1" t="s">
+    <row r="7" spans="2:2" ht="38.25">
+      <c r="B7" s="2" t="s">
         <v>147</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
-        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change the profiles in HCIMs HearingFunction and Stoma to use the new reasonReference extension on nl-core-observation
</commit_message>
<xml_diff>
--- a/Mappings/HearingFunction - STU3.xlsx
+++ b/Mappings/HearingFunction - STU3.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\nictiz-stu3-zib2017\Mappings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edelman\Nictiz-STU3-Zib2017\Mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{106EA0EF-58D7-47D2-926D-F5258AF1EBF4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -552,9 +553,6 @@
     <t>equal</t>
   </si>
   <si>
-    <t>.hearingAid -&gt; MedicalDevice (via extension http://nictiz.nl/fhir/StructureDefinition/extension-medicaldevice)</t>
-  </si>
-  <si>
     <t>MedicalDevice.device -&gt; MedicalDeviceProduct</t>
   </si>
   <si>
@@ -574,13 +572,16 @@
   </si>
   <si>
     <t>Observation (derived from nl-core-observation)</t>
+  </si>
+  <si>
+    <t>MedicalDevice</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
@@ -764,14 +765,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2919,18 +2920,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2938,7 +2939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -2946,7 +2947,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -2954,7 +2955,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
@@ -2962,7 +2963,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -2970,7 +2971,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
@@ -2978,7 +2979,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
@@ -2986,7 +2987,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
@@ -2994,7 +2995,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
@@ -3002,7 +3003,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
@@ -3010,7 +3011,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="38.25">
+    <row r="12" spans="2:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>55</v>
       </c>
@@ -3018,7 +3019,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="25.5">
+    <row r="13" spans="2:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>57</v>
       </c>
@@ -3026,7 +3027,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="2:3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>59</v>
       </c>
@@ -3036,7 +3037,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1"/>
+    <hyperlink ref="C11" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -3047,24 +3048,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="35" customWidth="1"/>
     <col min="3" max="3" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
-      <c r="B2" s="19" t="s">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="19"/>
-    </row>
-    <row r="3" spans="2:3">
+      <c r="C2" s="20"/>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
@@ -3072,7 +3073,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
@@ -3080,7 +3081,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
@@ -3088,7 +3089,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>26</v>
       </c>
@@ -3096,7 +3097,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
@@ -3104,7 +3105,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>28</v>
       </c>
@@ -3112,13 +3113,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="2:3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>31</v>
       </c>
@@ -3126,13 +3127,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="2:3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="2:3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
@@ -3140,13 +3141,13 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="2:3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="2:3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>37</v>
       </c>
@@ -3154,7 +3155,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="2:3">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>39</v>
       </c>
@@ -3162,7 +3163,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="2:3">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>41</v>
       </c>
@@ -3170,7 +3171,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>42</v>
       </c>
@@ -3178,7 +3179,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>43</v>
       </c>
@@ -3186,7 +3187,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>45</v>
       </c>
@@ -3194,7 +3195,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
         <v>46</v>
       </c>
@@ -3202,7 +3203,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="2:3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
         <v>47</v>
       </c>
@@ -3210,7 +3211,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="2:3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
         <v>49</v>
       </c>
@@ -3218,7 +3219,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
         <v>50</v>
       </c>
@@ -3226,7 +3227,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="2:3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
         <v>52</v>
       </c>
@@ -3234,7 +3235,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
         <v>53</v>
       </c>
@@ -3254,14 +3255,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
     </row>
   </sheetData>
@@ -3271,14 +3272,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="51.140625" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
@@ -3287,7 +3288,7 @@
     <col min="7" max="7" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>152</v>
       </c>
@@ -3305,7 +3306,7 @@
       <c r="G1" s="16"/>
       <c r="H1" s="16"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>156</v>
       </c>
@@ -3316,32 +3317,32 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>162</v>
       </c>
@@ -3352,7 +3353,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>163</v>
       </c>
@@ -3363,22 +3364,22 @@
         <v>167</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>178</v>
+      </c>
+      <c r="B17" s="19" t="s">
         <v>179</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>180</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B17" r:id="rId1" location="narrow/stream/179166-implementers/topic/Modeling.20Hearing.2FVisual.20Function" display="https://chat.fhir.org/ - narrow/stream/179166-implementers/topic/Modeling.20Hearing.2FVisual.20Function"/>
+    <hyperlink ref="B17" r:id="rId1" location="narrow/stream/179166-implementers/topic/Modeling.20Hearing.2FVisual.20Function" display="https://chat.fhir.org/ - narrow/stream/179166-implementers/topic/Modeling.20Hearing.2FVisual.20Function" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -3922,14 +3923,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="6" width="2" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
@@ -3945,7 +3946,7 @@
     <col min="19" max="19" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" ht="25.5">
+    <row r="2" spans="2:19" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
         <v>55</v>
       </c>
@@ -3991,7 +3992,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="3" spans="2:19" ht="38.25">
+    <row r="3" spans="2:19" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B3" s="8" t="s">
         <v>69</v>
       </c>
@@ -4017,15 +4018,15 @@
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
       <c r="P3" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
       <c r="S3" s="4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="4" spans="2:19" ht="25.5">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B4" s="11"/>
       <c r="C4" s="12" t="s">
         <v>69</v>
@@ -4069,7 +4070,7 @@
       </c>
       <c r="S4" s="3"/>
     </row>
-    <row r="5" spans="2:19" ht="51">
+    <row r="5" spans="2:19" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B5" s="11"/>
       <c r="C5" s="12" t="s">
         <v>82</v>
@@ -4101,13 +4102,13 @@
         <v>89</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
       <c r="S5" s="3"/>
     </row>
-    <row r="6" spans="2:19" ht="76.5">
+    <row r="6" spans="2:19" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
@@ -4137,7 +4138,7 @@
         <v>94</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Q6" s="2" t="s">
         <v>173</v>
@@ -4146,10 +4147,10 @@
         <v>2</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="7" spans="2:19" ht="38.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B7" s="11"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
@@ -4181,7 +4182,7 @@
         <v>100</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Q7" s="2" t="s">
         <v>173</v>
@@ -4191,7 +4192,7 @@
       </c>
       <c r="S7" s="3"/>
     </row>
-    <row r="8" spans="2:19" ht="25.5">
+    <row r="8" spans="2:19" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B8" s="11"/>
       <c r="C8" s="12" t="s">
         <v>101</v>
@@ -4233,10 +4234,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O4" location="HearingFunctionCodelist!A1" display="HearingFunctionCodelist"/>
-    <hyperlink ref="O5" r:id="rId1"/>
-    <hyperlink ref="O6" location="HearingAidTypeCodelist!A1" display="HearingAidTypeCodelist"/>
-    <hyperlink ref="O7" location="DeviceAnatomicalLocationCodelis!A1" display="DeviceAnatomicalLocationCodelist"/>
+    <hyperlink ref="O4" location="HearingFunctionCodelist!A1" display="HearingFunctionCodelist" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="O5" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="O6" location="HearingAidTypeCodelist!A1" display="HearingAidTypeCodelist" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="O7" location="DeviceAnatomicalLocationCodelis!A1" display="DeviceAnatomicalLocationCodelist" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -4247,12 +4248,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="C3:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -4261,18 +4262,18 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7">
-      <c r="C3" s="19" t="s">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19" t="s">
+      <c r="D3" s="20"/>
+      <c r="E3" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-    </row>
-    <row r="4" spans="3:7">
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C4" s="14" t="s">
         <v>109</v>
       </c>
@@ -4289,7 +4290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
         <v>113</v>
       </c>
@@ -4306,7 +4307,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="3:7">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
         <v>118</v>
       </c>
@@ -4323,7 +4324,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="3:7">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C7" s="2" t="s">
         <v>121</v>
       </c>
@@ -4353,12 +4354,12 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="C3:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -4367,18 +4368,18 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7">
-      <c r="C3" s="19" t="s">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19" t="s">
+      <c r="D3" s="20"/>
+      <c r="E3" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-    </row>
-    <row r="4" spans="3:7">
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C4" s="14" t="s">
         <v>109</v>
       </c>
@@ -4395,7 +4396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7" ht="25.5">
+    <row r="5" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
         <v>125</v>
       </c>
@@ -4412,7 +4413,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="3:7">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
         <v>129</v>
       </c>
@@ -4442,12 +4443,12 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="C3:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -4456,18 +4457,18 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7">
-      <c r="C3" s="19" t="s">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19" t="s">
+      <c r="D3" s="20"/>
+      <c r="E3" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-    </row>
-    <row r="4" spans="3:7">
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C4" s="14" t="s">
         <v>109</v>
       </c>
@@ -4484,7 +4485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
         <v>133</v>
       </c>
@@ -4501,7 +4502,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="3:7">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
         <v>136</v>
       </c>
@@ -4518,7 +4519,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="7" spans="3:7">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C7" s="2" t="s">
         <v>139</v>
       </c>
@@ -4548,42 +4549,42 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="B2:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="150" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="2:2" ht="140.25">
+    <row r="3" spans="2:2" ht="140.25" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="2:2">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="25.5">
+    <row r="5" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="6" spans="2:2">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="38.25">
+    <row r="7" spans="2:2" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>147</v>
       </c>

</xml_diff>